<commit_message>
Improved GUI, cleaned up heatCapacity.xlsx
</commit_message>
<xml_diff>
--- a/heatCapacity.xlsx
+++ b/heatCapacity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\MATLAB\heatCapEnthalpy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\MATLAB\Enthalpy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC9E52C-5362-4AE2-99C9-E4369A949777}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CD47D2-ED7E-4EBE-B9E1-330E4A1A780B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27720" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5745" yWindow="3045" windowWidth="14670" windowHeight="8415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -650,7 +650,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -708,7 +708,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -824,7 +824,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -882,7 +882,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -940,7 +940,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -969,7 +969,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>1357</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
@@ -1143,7 +1143,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>38</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>38</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>39</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>44</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>46</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>46</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>47</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>48</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>49</v>
       </c>
@@ -1750,7 +1750,7 @@
       </c>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>49</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>52</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>53</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>55</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>55</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>57</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>58</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>59</v>
       </c>
@@ -2096,7 +2096,7 @@
       </c>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>60</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>61</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>62</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>63</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>64</v>
       </c>

</xml_diff>